<commit_message>
Title: Capitalize words after colons. Accessed date: fixed date differences on AWS.
</commit_message>
<xml_diff>
--- a/static/Journal_names_map.xlsx
+++ b/static/Journal_names_map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Heart</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Lancet Neurology</t>
+  </si>
+  <si>
+    <t>Molecular Therapy : The Journal of the American Society of Gene Therapy</t>
+  </si>
+  <si>
+    <t>Molecular Therapy</t>
   </si>
 </sst>
 </file>
@@ -454,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCD6329-B956-4B64-8ED3-5136B910B9BD}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,6 +575,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Expanded map to clean more journal names
</commit_message>
<xml_diff>
--- a/static/Journal_names_map.xlsx
+++ b/static/Journal_names_map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>Heart</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Knee surgery, sports traumatology, arthroscopy : official journal of the ESSKA</t>
   </si>
   <si>
-    <t>Orthopaedics &amp; Traumatology, Surgery &amp; Research</t>
-  </si>
-  <si>
     <t>Orthopaedics &amp; traumatology, surgery &amp; research : OTSR</t>
   </si>
   <si>
@@ -108,6 +105,357 @@
   </si>
   <si>
     <t>Molecular Therapy</t>
+  </si>
+  <si>
+    <t>Arthritis &amp; Rheumatology (Hoboken, N.J.)</t>
+  </si>
+  <si>
+    <t>BMJ (Clinical Research Ed.)</t>
+  </si>
+  <si>
+    <t>BMJ</t>
+  </si>
+  <si>
+    <t>Canadian Family Physician Medecin De Famille Canadien</t>
+  </si>
+  <si>
+    <t>Canadian Family Physician</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Emergency Medicine</t>
+  </si>
+  <si>
+    <t>Cjem</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Gastroenterology = Journal Canadien De Gastroenterologie</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Gastroenterology</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Ophthalmology. Journal Canadien d'Ophtalmologie</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Ophthalmology</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Psychiatry. Revue Canadienne De Psychiatrie</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Psychiatry</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Public Health = Revue Canadienne De Sante Publique</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Public Health</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Rural Medicine : The Official Journal of the Society of Rural Physicians of Canada = Journal Canadien De La Medecine Rurale : Le Journal Officiel De La Societe De Medecine Rurale Du Canada</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Rural Medicine</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Surgery. Journal Canadien De Chirurgie</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Surgery</t>
+  </si>
+  <si>
+    <t>CMAJ : Canadian Medical Association Journal = Journal De l'Association Medicale Canadienne</t>
+  </si>
+  <si>
+    <t>Canadian Medical Association Journal</t>
+  </si>
+  <si>
+    <t>Canadian Urological Association Journal = Journal De l'Association Des Urologues Du Canada</t>
+  </si>
+  <si>
+    <t>Canadian Urological Association Journal</t>
+  </si>
+  <si>
+    <t>Health Promotion and Chronic Disease Prevention in Canada : Research, Policy and Practice</t>
+  </si>
+  <si>
+    <t>Health Promotion and Chronic Disease Prevention in Canada</t>
+  </si>
+  <si>
+    <t>Circulation. Cardiovascular Quality and Outcomes</t>
+  </si>
+  <si>
+    <t>Clinical Infectious Diseases : An Official Publication of the Infectious Diseases Society of America</t>
+  </si>
+  <si>
+    <t>Clinical Infectious Diseases</t>
+  </si>
+  <si>
+    <t>Health Affairs (Project Hope)</t>
+  </si>
+  <si>
+    <t>Health Affairs</t>
+  </si>
+  <si>
+    <t>Health Expectations : An International Journal of Public Participation in Health Care and Health Policy</t>
+  </si>
+  <si>
+    <t>Health Expectations</t>
+  </si>
+  <si>
+    <t>Jama</t>
+  </si>
+  <si>
+    <t>JAMA</t>
+  </si>
+  <si>
+    <t>Journal of Bone and Joint Surgery (American Volume)</t>
+  </si>
+  <si>
+    <t>The Journal of Bone and Joint Surgery. American Volume</t>
+  </si>
+  <si>
+    <t>Journal of Psychiatry &amp; Neuroscience : JPN</t>
+  </si>
+  <si>
+    <t>Medical Decision Making</t>
+  </si>
+  <si>
+    <t>Medical Decision Making : An International Journal of the Society for Medical Decision Making</t>
+  </si>
+  <si>
+    <t>Journal of Psychiatry and Neuroscience</t>
+  </si>
+  <si>
+    <t>The Medical Letter on Drugs and Therapeutics</t>
+  </si>
+  <si>
+    <t>Medical Letter on Drugs and Therapeutics</t>
+  </si>
+  <si>
+    <t>MMWR. Morbidity and Mortality Weekly Report</t>
+  </si>
+  <si>
+    <t>Morbidity and Mortality Weekly Report</t>
+  </si>
+  <si>
+    <t>The Orthopedic Clinics of North America</t>
+  </si>
+  <si>
+    <t>Orthopedic Clinics of North America</t>
+  </si>
+  <si>
+    <t>Circulation: Cardiovascular Quality and Outcomes</t>
+  </si>
+  <si>
+    <t>Circulation. Heart Failure</t>
+  </si>
+  <si>
+    <t>Circulation: Heart Failure</t>
+  </si>
+  <si>
+    <t>Journal of the American Society of Nephrology : JASN</t>
+  </si>
+  <si>
+    <t>Journal of the American Society of Nephrology</t>
+  </si>
+  <si>
+    <t>Genetics in Medicine : Official Journal of the American College of Medical Genetics</t>
+  </si>
+  <si>
+    <t>Genetics in Medicine</t>
+  </si>
+  <si>
+    <t>The American Journal of Clinical Nutrition</t>
+  </si>
+  <si>
+    <t>American Journal of Clinical Nutrition</t>
+  </si>
+  <si>
+    <t>Circulation. Cardiovascular Imaging</t>
+  </si>
+  <si>
+    <t>Circulation: Cardiovascular Imaging</t>
+  </si>
+  <si>
+    <t>Journal of Experimental Psychology. General</t>
+  </si>
+  <si>
+    <t>Journal of Experimental Psychology (General)</t>
+  </si>
+  <si>
+    <t>The European Respiratory Journal</t>
+  </si>
+  <si>
+    <t>European Respiratory Journal</t>
+  </si>
+  <si>
+    <t>The American Journal of Sports Medicine</t>
+  </si>
+  <si>
+    <t>American Journal of Sports Medicine</t>
+  </si>
+  <si>
+    <t>Small (Weinheim an Der Bergstrasse, Germany)</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Circulation. Arrhythmia and Electrophysiology</t>
+  </si>
+  <si>
+    <t>Circulation: Arrhythmia and Electrophysiology</t>
+  </si>
+  <si>
+    <t>Sports Medicine (Auckland, N.Z.)</t>
+  </si>
+  <si>
+    <t>Sports Medicine</t>
+  </si>
+  <si>
+    <t>The British Journal of Psychiatry : The Journal of Mental Science</t>
+  </si>
+  <si>
+    <t>British Journal of Psychiatry</t>
+  </si>
+  <si>
+    <t>Stem Cells (Dayton, Ohio)</t>
+  </si>
+  <si>
+    <t>Stem Cells</t>
+  </si>
+  <si>
+    <t>Rare Diseases (Austin, Tex.)</t>
+  </si>
+  <si>
+    <t>Rare Diseases</t>
+  </si>
+  <si>
+    <t>International Journal of Obesity (2005)</t>
+  </si>
+  <si>
+    <t>International Journal of Obesity (London)</t>
+  </si>
+  <si>
+    <t>Journal of Thoracic Oncology : Official Publication of the International Association for the Study of Lung Cancer</t>
+  </si>
+  <si>
+    <t>Journal of Thoracic Oncology</t>
+  </si>
+  <si>
+    <t>FASEB Journal : Official Publication of the Federation of American Societies for Experimental Biology</t>
+  </si>
+  <si>
+    <t>FASEB Journal</t>
+  </si>
+  <si>
+    <t>Journal of Thrombosis and Haemostasis : JTH</t>
+  </si>
+  <si>
+    <t>Journal of Thrombosis and Haemostasis</t>
+  </si>
+  <si>
+    <t>BMJ Quality &amp; Safety</t>
+  </si>
+  <si>
+    <t>BMJ Quality and Safety</t>
+  </si>
+  <si>
+    <t>Orthopaedics and Traumatology, Surgery and Research</t>
+  </si>
+  <si>
+    <t>Arthritis and Rheumatology</t>
+  </si>
+  <si>
+    <t>Cell Death &amp; Disease</t>
+  </si>
+  <si>
+    <t>Cell Death and Disease</t>
+  </si>
+  <si>
+    <t>Circulation. Cardiovascular Genetics</t>
+  </si>
+  <si>
+    <t>Circulation: Cardiovascular Genetics</t>
+  </si>
+  <si>
+    <t>Euro Surveillance : Bulletin Europeen Sur Les Maladies Transmissibles = European Communicable Disease Bulletin</t>
+  </si>
+  <si>
+    <t>Euro Surveillance</t>
+  </si>
+  <si>
+    <t>The International Journal of Behavioral Nutrition and Physical Activity</t>
+  </si>
+  <si>
+    <t>International Journal of Behavioral Nutrition and Physical Activity</t>
+  </si>
+  <si>
+    <t>The Journal of Clinical Psychiatry</t>
+  </si>
+  <si>
+    <t>Journal of Clinical Psychiatry</t>
+  </si>
+  <si>
+    <t>The Oncologist</t>
+  </si>
+  <si>
+    <t>Oncologist</t>
+  </si>
+  <si>
+    <t>Emotion (Washington, D.C.)</t>
+  </si>
+  <si>
+    <t>Emotion</t>
+  </si>
+  <si>
+    <t>Addiction (Abingdon, England)</t>
+  </si>
+  <si>
+    <t>Addiction</t>
+  </si>
+  <si>
+    <t>Academic Medicine : Journal of the Association of American Medical Colleges</t>
+  </si>
+  <si>
+    <t>Academic Medicine</t>
+  </si>
+  <si>
+    <t>Journal of Nuclear Medicine : Official Publication, Society of Nuclear Medicine</t>
+  </si>
+  <si>
+    <t>Journal of Nuclear Medicine</t>
+  </si>
+  <si>
+    <t>Critical Care (London, England)</t>
+  </si>
+  <si>
+    <t>Critical Care</t>
+  </si>
+  <si>
+    <t>Experimental &amp; Molecular Medicine</t>
+  </si>
+  <si>
+    <t>Experimental and Molecular Medicine</t>
+  </si>
+  <si>
+    <t>Obesity (Silver Spring, Md.)</t>
+  </si>
+  <si>
+    <t>Obesity</t>
+  </si>
+  <si>
+    <t>Journal of Psychopharmacology (Oxford, England)</t>
+  </si>
+  <si>
+    <t>Journal of Psychopharmacology</t>
+  </si>
+  <si>
+    <t>Cancer Immunology, Immunotherapy : CII</t>
+  </si>
+  <si>
+    <t>Cancer Immunology, Immunotherapy</t>
   </si>
 </sst>
 </file>
@@ -143,9 +491,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCD6329-B956-4B64-8ED3-5136B910B9BD}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,50 +830,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
+        <v>130</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>10</v>
+      <c r="A6" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
+        <v>110</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -537,53 +886,520 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
-        <v>27</v>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>138</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>90</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>94</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>98</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>80</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>88</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>86</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>120</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>122</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>124</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B72">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Clean up of comments in code
</commit_message>
<xml_diff>
--- a/static/Journal_names_map.xlsx
+++ b/static/Journal_names_map.xlsx
@@ -38,12 +38,6 @@
     <t>New England Journal of Medicine</t>
   </si>
   <si>
-    <t>HW_style</t>
-  </si>
-  <si>
-    <t>PubMed_name</t>
-  </si>
-  <si>
     <t>Nature reviews. Immunology</t>
   </si>
   <si>
@@ -462,6 +456,12 @@
   </si>
   <si>
     <t>Journal of the American Society of Hypertension</t>
+  </si>
+  <si>
+    <t>PubMed_title</t>
+  </si>
+  <si>
+    <t>Formatted_title</t>
   </si>
 </sst>
 </file>
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCD6329-B956-4B64-8ED3-5136B910B9BD}">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -828,282 +828,282 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -1116,274 +1116,274 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B53" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B67" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
@@ -1396,18 +1396,18 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arch of Otolaryngology--Head & Neck Surgery
</commit_message>
<xml_diff>
--- a/static/Journal_names_map.xlsx
+++ b/static/Journal_names_map.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chad\Dropbox\Data Box\Bella\zappa_app2\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B206D2-FD2E-4CDA-8A66-C6AA2A7935CA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6450" xr2:uid="{1B606881-0A46-4BDD-A0C9-1CF0B5D67379}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
   <si>
     <t>Heart</t>
   </si>
@@ -462,6 +463,12 @@
   </si>
   <si>
     <t>Formatted_title</t>
+  </si>
+  <si>
+    <t>Archives of Otolaryngology Head and Neck Surgery</t>
+  </si>
+  <si>
+    <t>Archives of otolaryngology--head &amp; neck surgery</t>
   </si>
 </sst>
 </file>
@@ -815,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCD6329-B956-4B64-8ED3-5136B910B9BD}">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -860,558 +867,566 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
+        <v>108</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>141</v>
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>113</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" t="s">
-        <v>71</v>
+        <v>80</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>73</v>
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
+        <v>72</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>132</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>133</v>
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" t="s">
-        <v>54</v>
+        <v>76</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>100</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>101</v>
+        <v>15</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B39" t="s">
-        <v>58</v>
+        <v>100</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>83</v>
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>130</v>
+        <v>82</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" t="s">
-        <v>64</v>
+        <v>130</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>138</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>139</v>
+        <v>61</v>
+      </c>
+      <c r="B44" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>142</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>75</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" t="s">
-        <v>18</v>
+        <v>106</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>67</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="B52" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>23</v>
-      </c>
-      <c r="B53" t="s">
-        <v>24</v>
+        <v>67</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>136</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>137</v>
+        <v>4</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>20</v>
-      </c>
-      <c r="B56" t="s">
-        <v>110</v>
+        <v>136</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>98</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>99</v>
+        <v>20</v>
+      </c>
+      <c r="B57" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>10</v>
-      </c>
-      <c r="B64" t="s">
-        <v>11</v>
+        <v>94</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>85</v>
+        <v>10</v>
+      </c>
+      <c r="B65" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B67" t="s">
-        <v>59</v>
+        <v>118</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>120</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>121</v>
+        <v>60</v>
+      </c>
+      <c r="B68" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>21</v>
-      </c>
-      <c r="B69" t="s">
-        <v>22</v>
+        <v>120</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>122</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>122</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B73">
+  <sortState ref="A2:B74">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
NLP to detect Title Case and convert to Sentence case
</commit_message>
<xml_diff>
--- a/static/Journal_names_map.xlsx
+++ b/static/Journal_names_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chad\Dropbox\Data Box\Bella\zappa_app2\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B206D2-FD2E-4CDA-8A66-C6AA2A7935CA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C37F54-428C-4F27-9988-94FA412115CF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6450" xr2:uid="{1B606881-0A46-4BDD-A0C9-1CF0B5D67379}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>Heart</t>
   </si>
@@ -469,6 +469,12 @@
   </si>
   <si>
     <t>Archives of otolaryngology--head &amp; neck surgery</t>
+  </si>
+  <si>
+    <t>Journal of Obstetrics and Gynaecology Canada</t>
+  </si>
+  <si>
+    <t>Journal of obstetrics and gynaecology Canada : JOGC = Journal d'obstetrique et gynecologie du Canada : JOGC</t>
   </si>
 </sst>
 </file>
@@ -822,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCD6329-B956-4B64-8ED3-5136B910B9BD}">
-  <dimension ref="A1:B74"/>
+  <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1179,254 +1185,262 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" t="s">
-        <v>64</v>
+        <v>149</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>138</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>139</v>
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>142</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>75</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>19</v>
-      </c>
-      <c r="B50" t="s">
-        <v>18</v>
+        <v>106</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>67</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="B53" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>23</v>
-      </c>
-      <c r="B54" t="s">
-        <v>24</v>
+        <v>67</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>136</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>137</v>
+        <v>4</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>20</v>
-      </c>
-      <c r="B57" t="s">
-        <v>110</v>
+        <v>136</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>98</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>99</v>
+        <v>20</v>
+      </c>
+      <c r="B58" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>10</v>
-      </c>
-      <c r="B65" t="s">
-        <v>11</v>
+        <v>94</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>84</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>85</v>
+        <v>10</v>
+      </c>
+      <c r="B66" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>60</v>
-      </c>
-      <c r="B68" t="s">
-        <v>59</v>
+        <v>118</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>120</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>121</v>
+        <v>60</v>
+      </c>
+      <c r="B69" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>21</v>
-      </c>
-      <c r="B70" t="s">
-        <v>22</v>
+        <v>120</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
+        <v>21</v>
+      </c>
+      <c r="B71" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>65</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>122</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
+        <v>122</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B74">
+  <sortState ref="A1:B75">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Am J Transplantation to journals map
</commit_message>
<xml_diff>
--- a/static/Journal_names_map.xlsx
+++ b/static/Journal_names_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chad\Dropbox\Data Box\Bella\zappa_app2\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chad\Documents\Work\Data science\Apps\Bella\app\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C37F54-428C-4F27-9988-94FA412115CF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB4794F-3AA3-40A6-855C-9BE3ACD3E7E9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6450" xr2:uid="{1B606881-0A46-4BDD-A0C9-1CF0B5D67379}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>Heart</t>
   </si>
@@ -475,6 +475,12 @@
   </si>
   <si>
     <t>Journal of obstetrics and gynaecology Canada : JOGC = Journal d'obstetrique et gynecologie du Canada : JOGC</t>
+  </si>
+  <si>
+    <t>American Journal of Transplantation : Official Journal of the American Society of Transplantation and the American Society of Transplant Surgeons</t>
+  </si>
+  <si>
+    <t>American Journal of Transplantation</t>
   </si>
 </sst>
 </file>
@@ -828,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCD6329-B956-4B64-8ED3-5136B910B9BD}">
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1439,6 +1445,14 @@
         <v>70</v>
       </c>
     </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:B75">
     <sortCondition ref="A2"/>

</xml_diff>